<commit_message>
fixing project for design analysis
</commit_message>
<xml_diff>
--- a/WI 24/SE 160A/MATLAB PROJECT 1 TEST/2024_SE160A_MATLAB_Spar_Student_Project/2024_SE160A_MATLAB_Spar_Student_Project/SE160A_1_Spar_Analysis_Input.xlsx
+++ b/WI 24/SE 160A/MATLAB PROJECT 1 TEST/2024_SE160A_MATLAB_Spar_Student_Project/2024_SE160A_MATLAB_Spar_Student_Project/SE160A_1_Spar_Analysis_Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levih\OneDrive\Documents\GitHub\UCSD\WI 24\SE 160A\MATLAB PROJECT 1 TEST\2024_SE160A_MATLAB_Spar_Student_Project\2024_SE160A_MATLAB_Spar_Student_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000EC98D-4BEC-43A9-9D09-50680BBA44B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E5BEC1-773A-441D-B6A3-2D606CEAB64E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2412,7 +2412,7 @@
   </sheetPr>
   <dimension ref="A1:R60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D17" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
@@ -2969,10 +2969,10 @@
         <v>92</v>
       </c>
       <c r="G39" s="29">
-        <v>0</v>
+        <v>0.2555</v>
       </c>
       <c r="H39" s="29">
-        <v>0</v>
+        <v>0.75549999999999995</v>
       </c>
       <c r="I39" s="11">
         <v>1</v>
@@ -2991,10 +2991,10 @@
         <v>88</v>
       </c>
       <c r="G40" s="98">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H40" s="98">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I40" s="85" t="s">
         <v>89</v>
@@ -3013,10 +3013,10 @@
         <v>90</v>
       </c>
       <c r="G41" s="98">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="H41" s="98">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="I41" s="85" t="s">
         <v>89</v>
@@ -3035,10 +3035,10 @@
         <v>91</v>
       </c>
       <c r="G42" s="98">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H42" s="98">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I42" s="85" t="s">
         <v>89</v>
@@ -3057,10 +3057,10 @@
         <v>100</v>
       </c>
       <c r="G43" s="98">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="H43" s="98">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="I43" s="85" t="s">
         <v>113</v>
@@ -3079,10 +3079,10 @@
         <v>101</v>
       </c>
       <c r="G44" s="98">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H44" s="98">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I44" s="85" t="s">
         <v>113</v>
@@ -3101,10 +3101,10 @@
         <v>102</v>
       </c>
       <c r="G45" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H45" s="30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I45" s="86" t="s">
         <v>113</v>

</xml_diff>